<commit_message>
add complete scraping of halyard health and gtins for gloves
</commit_message>
<xml_diff>
--- a/tcesr-template.xlsx
+++ b/tcesr-template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -893,8 +893,8 @@
   </sheetPr>
   <dimension ref="A1:Z265"/>
   <sheetViews>
-    <sheetView topLeftCell="L18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5972,7 +5972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O18"/>
     </sheetView>
   </sheetViews>

</xml_diff>